<commit_message>
Standardize some naming and formatting
</commit_message>
<xml_diff>
--- a/Cell wall composition and Stomatal density/CGR3 greenhouse stomatal density and cell wall analysis.xlsx
+++ b/Cell wall composition and Stomatal density/CGR3 greenhouse stomatal density and cell wall analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGB\Documents\GitHub\CGR3-tobacco-2024\Cell wall composition and Stomatal density\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eloch\Documents\GitHub\CGR3-tobacco-2024\Cell wall composition and Stomatal density\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3525" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3528" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cell wall analysis" sheetId="1" r:id="rId1"/>
@@ -111,56 +111,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -181,62 +154,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,50 +469,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="J1" s="4" t="s">
@@ -576,1034 +525,1034 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
         <v>14</v>
       </c>
-      <c r="B2" s="7">
-        <v>8</v>
-      </c>
-      <c r="C2" s="8">
+      <c r="B2" s="8">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9">
         <v>52.069607537356354</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>16.427738890761944</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>156.66598039648514</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="9">
         <v>128.02000000000001</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="9">
         <v>66.89</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="10">
         <f t="shared" ref="H2:H25" si="0">(E2+G2)/F2</f>
         <v>1.7462582439969156</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="11">
         <f>E2+G2</f>
         <v>223.55598039648515</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="10">
         <f t="shared" ref="J2:J25" si="1">F2/(E2+G2)</f>
         <v>0.57265298728735237</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="10">
         <f t="shared" ref="K2:K25" si="2">E2+F2+G2</f>
         <v>351.57598039648514</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="9">
         <f>C2/D2</f>
         <v>3.1696149959284678</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
         <v>14</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="8">
         <v>6</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="9">
         <v>55.420888383247927</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>25.301486226777712</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>166.77882251832625</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="9">
         <v>67.19</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="9">
         <v>80.650000000000006</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="10">
         <f t="shared" si="0"/>
         <v>3.6825245202906127</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="11">
         <f t="shared" ref="I3:I25" si="3">E3+G3</f>
         <v>247.42882251832626</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="10">
         <f t="shared" si="1"/>
         <v>0.27155284221191917</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="10">
         <f t="shared" si="2"/>
         <v>314.61882251832628</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="9">
         <f t="shared" ref="L3:L25" si="4">C3/D3</f>
         <v>2.1904202735961609</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
         <v>14</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
         <v>5</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="9">
         <v>50.647415408066266</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>45.735542277747598</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>168.74825460448861</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="9">
         <v>54.19</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="9">
         <v>60.28</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="10">
         <f t="shared" si="0"/>
         <v>4.2263933309556858</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="11">
         <f t="shared" si="3"/>
         <v>229.02825460448861</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="10">
         <f t="shared" si="1"/>
         <v>0.23660836124163501</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="10">
         <f t="shared" si="2"/>
         <v>283.21825460448861</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="9">
         <f t="shared" si="4"/>
         <v>1.1073972863487511</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
         <v>14</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="8">
         <v>4</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="9">
         <v>45.277724306882021</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <v>29.976550561797747</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>157.61137809495747</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="9">
         <v>48.19</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="9">
         <v>61.51</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="10">
         <f t="shared" si="0"/>
         <v>4.5470300496982254</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="11">
         <f t="shared" si="3"/>
         <v>219.12137809495746</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="10">
         <f t="shared" si="1"/>
         <v>0.21992377201605859</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="10">
         <f t="shared" si="2"/>
         <v>267.31137809495749</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="9">
         <f t="shared" si="4"/>
         <v>1.5104381077315867</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <v>14</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="9">
         <v>43.772047638695042</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>26.144615026750412</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <v>136.70494326308176</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="9">
         <v>47.58</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="9">
         <v>71.2</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="10">
         <f t="shared" si="0"/>
         <v>4.3695868697579181</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="11">
         <f t="shared" si="3"/>
         <v>207.90494326308175</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="10">
         <f t="shared" si="1"/>
         <v>0.22885458735722572</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="10">
         <f t="shared" si="2"/>
         <v>255.48494326308173</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="9">
         <f t="shared" si="4"/>
         <v>1.6742280425207543</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>14</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>2</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="9">
         <v>59.174926430839321</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>33.967318240382859</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>169.25333475938876</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="9">
         <v>68.98</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="9">
         <v>49.11</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="10">
         <f t="shared" si="0"/>
         <v>3.1656035772599123</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="11">
         <f t="shared" si="3"/>
         <v>218.36333475938875</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="10">
         <f t="shared" si="1"/>
         <v>0.3158955237426101</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="10">
         <f t="shared" si="2"/>
         <v>287.34333475938877</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="9">
         <f t="shared" si="4"/>
         <v>1.7421135814156736</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>10</v>
-      </c>
-      <c r="B8" s="12">
-        <v>10</v>
-      </c>
-      <c r="C8" s="13">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9">
         <v>58.638976458887704</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="9">
         <v>29.328681923008688</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="9">
         <v>131.26431068026668</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="9">
         <v>89.12</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="9">
         <v>50.64</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="10">
         <f t="shared" si="0"/>
         <v>2.0411165920137644</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="11">
         <f t="shared" si="3"/>
         <v>181.90431068026669</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="10">
         <f t="shared" si="1"/>
         <v>0.48992791686309334</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="10">
         <f t="shared" si="2"/>
         <v>271.02431068026669</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="9">
         <f t="shared" si="4"/>
         <v>1.9993730578422195</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>10</v>
-      </c>
-      <c r="B9" s="12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>10</v>
+      </c>
+      <c r="B9" s="8">
         <v>9</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="9">
         <v>58.534585547907504</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="9">
         <v>39.690450318159563</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="9">
         <v>135.14421164594637</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="9">
         <v>56.31</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="9">
         <v>60.51</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="10">
         <f t="shared" si="0"/>
         <v>3.4745908656712192</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="11">
         <f t="shared" si="3"/>
         <v>195.65421164594636</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="10">
         <f t="shared" si="1"/>
         <v>0.28780366916863481</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="10">
         <f t="shared" si="2"/>
         <v>251.96421164594636</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="9">
         <f t="shared" si="4"/>
         <v>1.4747775618238876</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>10</v>
-      </c>
-      <c r="B10" s="12">
-        <v>8</v>
-      </c>
-      <c r="C10" s="13">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>10</v>
+      </c>
+      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9">
         <v>84.26620242409868</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="9">
         <v>41.765131773139366</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="9">
         <v>207.93207703237738</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="9">
         <v>55.95</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="9">
         <v>51.84</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="10">
         <f t="shared" si="0"/>
         <v>4.6429325653686755</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="11">
         <f t="shared" si="3"/>
         <v>259.77207703237741</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="10">
         <f t="shared" si="1"/>
         <v>0.21538111655097758</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="10">
         <f t="shared" si="2"/>
         <v>315.72207703237734</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="9">
         <f t="shared" si="4"/>
         <v>2.017620892035429</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>10</v>
-      </c>
-      <c r="B11" s="12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
         <v>4</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="9">
         <v>62.209762890672323</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="9">
         <v>33.506137694326661</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="9">
         <v>128.68374696341127</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="9">
         <v>65.67</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="9">
         <v>39.67</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="10">
         <f t="shared" si="0"/>
         <v>2.5636325104828881</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="11">
         <f t="shared" si="3"/>
         <v>168.35374696341125</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="10">
         <f t="shared" si="1"/>
         <v>0.39007150826451298</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="10">
         <f t="shared" si="2"/>
         <v>234.02374696341127</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="9">
         <f t="shared" si="4"/>
         <v>1.8566676785670175</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8">
         <v>3</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="9">
         <v>64.125444605126887</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="9">
         <v>47.628489556361124</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="9">
         <v>108.2399611226558</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="9">
         <v>62.48</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="9">
         <v>39.630000000000003</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="10">
         <f t="shared" si="0"/>
         <v>2.3666767145111365</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="11">
         <f t="shared" si="3"/>
         <v>147.86996112265581</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="10">
         <f t="shared" si="1"/>
         <v>0.42253341737321359</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="10">
         <f t="shared" si="2"/>
         <v>210.3499611226558</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="9">
         <f t="shared" si="4"/>
         <v>1.3463673780635874</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>10</v>
-      </c>
-      <c r="B13" s="12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>10</v>
+      </c>
+      <c r="B13" s="8">
         <v>1</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <v>46.988141899262416</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="9">
         <v>21.233157349896484</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="9">
         <v>111.37421664559379</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="9">
         <v>84.14</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="9">
         <v>43.28</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="10">
         <f t="shared" si="0"/>
         <v>1.8380581964059164</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="11">
         <f t="shared" si="3"/>
         <v>154.65421664559381</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="10">
         <f t="shared" si="1"/>
         <v>0.5440524146381055</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="10">
         <f t="shared" si="2"/>
         <v>238.79421664559379</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="9">
         <f t="shared" si="4"/>
         <v>2.2129606598281764</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>8</v>
-      </c>
-      <c r="B14" s="14">
-        <v>10</v>
-      </c>
-      <c r="C14" s="15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9">
         <v>39.829503231691596</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="9">
         <v>37.682833075468452</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="9">
         <v>125.89415175547406</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="9">
         <v>84.21</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="9">
         <v>44.15</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="10">
         <f t="shared" si="0"/>
         <v>2.0192869226395209</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="11">
         <f t="shared" si="3"/>
         <v>170.04415175547405</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="10">
         <f t="shared" si="1"/>
         <v>0.4952243233927574</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="10">
         <f t="shared" si="2"/>
         <v>254.25415175547406</v>
       </c>
-      <c r="L14" s="11">
+      <c r="L14" s="9">
         <f t="shared" si="4"/>
         <v>1.0569667931263009</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>8</v>
-      </c>
-      <c r="B15" s="14">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>8</v>
+      </c>
+      <c r="B15" s="8">
         <v>9</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="9">
         <v>85.012288186257095</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="9">
         <v>26.981770833333332</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="9">
         <v>136.15532971988591</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="9">
         <v>85.76</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="9">
         <v>45.35</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="10">
         <f t="shared" si="0"/>
         <v>2.1164334155770277</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="11">
         <f t="shared" si="3"/>
         <v>181.50532971988591</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="10">
         <f t="shared" si="1"/>
         <v>0.47249301236692032</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="10">
         <f t="shared" si="2"/>
         <v>267.26532971988593</v>
       </c>
-      <c r="L15" s="11">
+      <c r="L15" s="9">
         <f t="shared" si="4"/>
         <v>3.1507304954659516</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>8</v>
-      </c>
-      <c r="B16" s="14">
-        <v>8</v>
-      </c>
-      <c r="C16" s="15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>8</v>
+      </c>
+      <c r="B16" s="8">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9">
         <v>66.300012895191699</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="9">
         <v>25.88054054054054</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="9">
         <v>133.08158336272629</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="9">
         <v>83</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="9">
         <v>56.22</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="10">
         <f t="shared" si="0"/>
         <v>2.2807419682256178</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="11">
         <f t="shared" si="3"/>
         <v>189.30158336272629</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="10">
         <f t="shared" si="1"/>
         <v>0.4384538075466663</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="10">
         <f t="shared" si="2"/>
         <v>272.30158336272632</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="9">
         <f t="shared" si="4"/>
         <v>2.5617707942125909</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
-        <v>8</v>
-      </c>
-      <c r="B17" s="14">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>8</v>
+      </c>
+      <c r="B17" s="8">
         <v>5</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="9">
         <v>63.748264068133636</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="9">
         <v>29.405440084835632</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="9">
         <v>121.14365314290853</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="9">
         <v>83.62</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="9">
         <v>76.39</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="10">
         <f t="shared" si="0"/>
         <v>2.3622776027614028</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="11">
         <f t="shared" si="3"/>
         <v>197.53365314290852</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="10">
         <f t="shared" si="1"/>
         <v>0.42332027312583509</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="10">
         <f t="shared" si="2"/>
         <v>281.15365314290852</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="9">
         <f t="shared" si="4"/>
         <v>2.1679071588188399</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <v>8</v>
-      </c>
-      <c r="B18" s="14">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>8</v>
+      </c>
+      <c r="B18" s="8">
         <v>3</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="9">
         <v>94.687732031511445</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="9">
         <v>40.380304889384639</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="9">
         <v>186.83455266203376</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="9">
         <v>72.84</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="9">
         <v>41.37</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="10">
         <f t="shared" si="0"/>
         <v>3.1329565165023854</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="11">
         <f t="shared" si="3"/>
         <v>228.20455266203376</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="10">
         <f t="shared" si="1"/>
         <v>0.31918732185801107</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="10">
         <f t="shared" si="2"/>
         <v>301.04455266203377</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="9">
         <f t="shared" si="4"/>
         <v>2.3448988879824775</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>8</v>
-      </c>
-      <c r="B19" s="14">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>8</v>
+      </c>
+      <c r="B19" s="8">
         <v>2</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="9">
         <v>61.422636480905865</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="9">
         <v>33.353360963094531</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="9">
         <v>161.97976793517765</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="9">
         <v>88.12</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="9">
         <v>44.71</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="10">
         <f t="shared" si="0"/>
         <v>2.3455488871445489</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="11">
         <f t="shared" si="3"/>
         <v>206.68976793517766</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="10">
         <f t="shared" si="1"/>
         <v>0.42633944041021093</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="10">
         <f t="shared" si="2"/>
         <v>294.80976793517766</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="9">
         <f t="shared" si="4"/>
         <v>1.841572624386189</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="8">
         <v>9</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="9">
         <v>56.688529339528401</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="9">
         <v>18.211700487128237</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="9">
         <v>148.53500865176738</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="9">
         <v>101.97</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="9">
         <v>52.29</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="10">
         <f t="shared" si="0"/>
         <v>1.9694518843950906</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="11">
         <f t="shared" si="3"/>
         <v>200.82500865176738</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="10">
         <f t="shared" si="1"/>
         <v>0.50775548665264603</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="10">
         <f t="shared" si="2"/>
         <v>302.79500865176738</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="9">
         <f t="shared" si="4"/>
         <v>3.1127532203593522</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="8">
         <v>7</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="9">
         <v>37.72262867734198</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="9">
         <v>23.533318284424382</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="9">
         <v>180.21697660791736</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="9">
         <v>112.01</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="9">
         <v>52.19</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="10">
         <f t="shared" si="0"/>
         <v>2.0748770342640599</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="11">
         <f t="shared" si="3"/>
         <v>232.40697660791736</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="10">
         <f t="shared" si="1"/>
         <v>0.48195627185911333</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="10">
         <f t="shared" si="2"/>
         <v>344.41697660791738</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="9">
         <f t="shared" si="4"/>
         <v>1.6029455863990438</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="8">
         <v>6</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="9">
         <v>46.811992764662605</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="9">
         <v>22.419904875148632</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="9">
         <v>139.66554715594705</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="9">
         <v>86.16</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G22" s="9">
         <v>60.69</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="10">
         <f t="shared" si="0"/>
         <v>2.3253893588201842</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="11">
         <f t="shared" si="3"/>
         <v>200.35554715594705</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="10">
         <f t="shared" si="1"/>
         <v>0.4300355104864515</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="10">
         <f t="shared" si="2"/>
         <v>286.51554715594705</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="9">
         <f t="shared" si="4"/>
         <v>2.0879657173100412</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="8">
         <v>4</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="9">
         <v>50.973462893723941</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="9">
         <v>23.73136948209941</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="9">
         <v>148.45656793662008</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="9">
         <v>87.03</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="9">
         <v>50.09</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="10">
         <f t="shared" si="0"/>
         <v>2.2813577839436983</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="11">
         <f t="shared" si="3"/>
         <v>198.54656793662008</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="10">
         <f t="shared" si="1"/>
         <v>0.43833545401692198</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="10">
         <f t="shared" si="2"/>
         <v>285.57656793662011</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="9">
         <f t="shared" si="4"/>
         <v>2.1479360022679375</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="8">
         <v>3</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="9">
         <v>62.497208922383713</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="9">
         <v>30.583304972584614</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="9">
         <v>173.44100303607465</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="9">
         <v>69.239999999999995</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="9">
         <v>48.88</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="10">
         <f t="shared" si="0"/>
         <v>3.2108752604863469</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="11">
         <f t="shared" si="3"/>
         <v>222.32100303607464</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="10">
         <f t="shared" si="1"/>
         <v>0.31144155997157341</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="10">
         <f t="shared" si="2"/>
         <v>291.56100303607462</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="9">
         <f t="shared" si="4"/>
         <v>2.0435073638512011</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="8">
         <v>2</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="9">
         <v>28.804637746489984</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="9">
         <v>16.662874743326491</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="9">
         <v>152.48186404664514</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="9">
         <v>64.98</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="9">
         <v>61.21</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="10">
         <f t="shared" si="0"/>
         <v>3.2885790096436618</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="11">
         <f t="shared" si="3"/>
         <v>213.69186404664515</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="10">
         <f t="shared" si="1"/>
         <v>0.30408270473889459</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="10">
         <f t="shared" si="2"/>
         <v>278.67186404664511</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="9">
         <f t="shared" si="4"/>
         <v>1.7286715641925046</v>
       </c>
@@ -1617,71 +1566,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="9" max="10" width="20.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="9" max="10" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1739,7 +1688,7 @@
         <v>2.2063492063492069</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8</v>
       </c>
@@ -1794,7 +1743,7 @@
         <v>2.3037974683544307</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -1849,7 +1798,7 @@
         <v>2.641509433962264</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -1904,7 +1853,7 @@
         <v>2.0909090909090913</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1959,7 +1908,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8</v>
       </c>
@@ -2014,7 +1963,7 @@
         <v>2.0666666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2069,7 +2018,7 @@
         <v>2.418181818181818</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2124,7 +2073,7 @@
         <v>2.1690140845070425</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2179,7 +2128,7 @@
         <v>1.9868421052631577</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2234,7 +2183,7 @@
         <v>2.9516129032258065</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2289,7 +2238,7 @@
         <v>2.704225352112676</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2344,7 +2293,7 @@
         <v>1.9295774647887325</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
@@ -2399,7 +2348,7 @@
         <v>1.6571428571428573</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -2454,7 +2403,7 @@
         <v>2.7708333333333326</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -2509,7 +2458,7 @@
         <v>2.0487804878048781</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8</v>
       </c>
@@ -2564,7 +2513,7 @@
         <v>2.166666666666667</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -2619,7 +2568,7 @@
         <v>2.1159420289855073</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8</v>
       </c>
@@ -2674,7 +2623,7 @@
         <v>2.4507042253521125</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>8</v>
       </c>
@@ -2729,7 +2678,7 @@
         <v>2.0350877192982457</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>8</v>
       </c>
@@ -2784,7 +2733,7 @@
         <v>2.3793103448275863</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>8</v>
       </c>
@@ -2839,7 +2788,7 @@
         <v>2.3787878787878789</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>8</v>
       </c>
@@ -2868,7 +2817,7 @@
         <v>0.46341463414634143</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8</v>
       </c>
@@ -2897,7 +2846,7 @@
         <v>0.45945945945945948</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2926,7 +2875,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -2955,7 +2904,7 @@
         <v>0.37500000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -2984,7 +2933,7 @@
         <v>0.44117647058823528</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
@@ -3013,7 +2962,7 @@
         <v>0.38235294117647062</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>10</v>
       </c>
@@ -3042,7 +2991,7 @@
         <v>0.45454545454545447</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>10</v>
       </c>
@@ -3071,7 +3020,7 @@
         <v>0.45945945945945948</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>10</v>
       </c>
@@ -3100,7 +3049,7 @@
         <v>0.39024390243902435</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>10</v>
       </c>
@@ -3129,7 +3078,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10</v>
       </c>
@@ -3158,7 +3107,7 @@
         <v>0.41463414634146339</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10</v>
       </c>
@@ -3187,7 +3136,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10</v>
       </c>
@@ -3216,7 +3165,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>10</v>
       </c>
@@ -3245,7 +3194,7 @@
         <v>0.55882352941176461</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>10</v>
       </c>
@@ -3274,7 +3223,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>10</v>
       </c>
@@ -3303,7 +3252,7 @@
         <v>0.39130434782608697</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10</v>
       </c>
@@ -3332,7 +3281,7 @@
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10</v>
       </c>
@@ -3361,7 +3310,7 @@
         <v>0.41463414634146339</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10</v>
       </c>
@@ -3390,7 +3339,7 @@
         <v>0.27659574468085107</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10</v>
       </c>
@@ -3419,7 +3368,7 @@
         <v>0.3529411764705882</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>10</v>
       </c>
@@ -3448,7 +3397,7 @@
         <v>0.32075471698113206</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>10</v>
       </c>
@@ -3477,7 +3426,7 @@
         <v>0.36956521739130438</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>10</v>
       </c>
@@ -3506,7 +3455,7 @@
         <v>0.45238095238095233</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>10</v>
       </c>
@@ -3535,7 +3484,7 @@
         <v>0.52941176470588236</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -3564,7 +3513,7 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10</v>
       </c>
@@ -3593,7 +3542,7 @@
         <v>0.48484848484848475</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10</v>
       </c>
@@ -3622,7 +3571,7 @@
         <v>0.47368421052631582</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>14</v>
       </c>
@@ -3651,7 +3600,7 @@
         <v>0.4838709677419355</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>14</v>
       </c>
@@ -3680,7 +3629,7 @@
         <v>0.69565217391304346</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>14</v>
       </c>
@@ -3709,7 +3658,7 @@
         <v>0.76923076923076916</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>14</v>
       </c>
@@ -3738,7 +3687,7 @@
         <v>0.52777777777777779</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>14</v>
       </c>
@@ -3767,7 +3716,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>14</v>
       </c>
@@ -3796,7 +3745,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>14</v>
       </c>
@@ -3825,7 +3774,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>14</v>
       </c>
@@ -3854,7 +3803,7 @@
         <v>0.38709677419354843</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>14</v>
       </c>
@@ -3883,7 +3832,7 @@
         <v>0.47619047619047622</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>14</v>
       </c>
@@ -3912,7 +3861,7 @@
         <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>14</v>
       </c>
@@ -3941,7 +3890,7 @@
         <v>0.44999999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>14</v>
       </c>
@@ -3970,7 +3919,7 @@
         <v>0.48780487804878048</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>14</v>
       </c>
@@ -3999,7 +3948,7 @@
         <v>0.39473684210526316</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>14</v>
       </c>
@@ -4028,7 +3977,7 @@
         <v>0.47058823529411759</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>14</v>
       </c>
@@ -4057,7 +4006,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>14</v>
       </c>
@@ -4086,7 +4035,7 @@
         <v>0.48571428571428571</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>14</v>
       </c>
@@ -4115,7 +4064,7 @@
         <v>0.34883720930232559</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>14</v>
       </c>
@@ -4144,7 +4093,7 @@
         <v>0.47058823529411759</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>14</v>
       </c>
@@ -4173,7 +4122,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>14</v>
       </c>
@@ -4202,7 +4151,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -4231,7 +4180,7 @@
         <v>0.44680851063829785</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -4260,7 +4209,7 @@
         <v>0.45945945945945948</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -4289,7 +4238,7 @@
         <v>0.36170212765957449</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -4318,7 +4267,7 @@
         <v>0.37209302325581395</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -4347,7 +4296,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -4376,7 +4325,7 @@
         <v>0.44827586206896558</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -4405,7 +4354,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>6</v>
       </c>
@@ -4434,7 +4383,7 @@
         <v>0.51724137931034486</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -4463,7 +4412,7 @@
         <v>0.45454545454545447</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -4492,7 +4441,7 @@
         <v>0.41176470588235292</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -4521,7 +4470,7 @@
         <v>0.42105263157894735</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -4550,7 +4499,7 @@
         <v>0.39393939393939392</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>6</v>
       </c>
@@ -4579,7 +4528,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>6</v>
       </c>
@@ -4608,7 +4557,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>6</v>
       </c>
@@ -4637,7 +4586,7 @@
         <v>0.42105263157894735</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>6</v>
       </c>

</xml_diff>